<commit_message>
second round of data
</commit_message>
<xml_diff>
--- a/Data/ScienceFair2025-Data.xlsx
+++ b/Data/ScienceFair2025-Data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mct\Katie-ScienceFair-2025\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{650A2462-41F9-4518-BCFF-0F10A189221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BEDBCE-DEC2-451E-887A-331C5650BC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{FFB2D0E0-05BF-4FD5-8F8B-8FC4333E2434}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="2" xr2:uid="{FFB2D0E0-05BF-4FD5-8F8B-8FC4333E2434}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Measurements" sheetId="2" r:id="rId2"/>
+    <sheet name="Measurements (2)" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>RSSI</t>
   </si>
@@ -162,20 +162,38 @@
   <si>
     <t>no box</t>
   </si>
+  <si>
+    <t>11 cm.</t>
+  </si>
+  <si>
+    <t>12 cm.</t>
+  </si>
+  <si>
+    <t>13 cm.</t>
+  </si>
+  <si>
+    <t>14 cm.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="0.000000"/>
-    <numFmt numFmtId="172" formatCode="0.0000000"/>
-    <numFmt numFmtId="173" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,12 +219,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,6 +946,804 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10735542893990459"/>
+          <c:y val="0.18560185185185185"/>
+          <c:w val="0.85794207585855986"/>
+          <c:h val="0.72125801983085447"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurements (2)'!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power (W)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurements (2)'!$A$27:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurements (2)'!$C$27:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6.5313055264747098E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3489628825916523E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1622776601683783E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4621771744567172E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2022644346174124E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6885293084384106E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6788040181225605E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3442288153199212E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6238102139926025E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3282453313890383E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.0794578438413788E-2</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.0000000">
+                  <c:v>0.10115794542598987</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.0000000">
+                  <c:v>7.2443596007498959E-2</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0000000">
+                  <c:v>9.8855309465693833E-2</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.0000000">
+                  <c:v>8.2224264994707086E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.03526122185617E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-56F3-40E7-B3C0-014AAACD7728}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="79852655"/>
+        <c:axId val="79853615"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="79852655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79853615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="79853615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79852655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.3407992906836736E-2"/>
+          <c:y val="0.18097222222222226"/>
+          <c:w val="0.8918895118916278"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Measurements (2)'!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dBm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Measurements (2)'!$A$27:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Measurements (2)'!$B$27:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-51.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-28.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-38.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-29.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-22.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-17.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-16.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-13.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-11.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-11.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-9.9499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-11.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-10.050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-10.85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-10.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FBC3-401D-A39F-A6CAE9E1DFD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1384472703"/>
+        <c:axId val="1384473183"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1384472703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1384473183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1384473183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1384472703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -999,6 +1824,52 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1516,6 +2387,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2092,6 +3995,87 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>473867</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>140492</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BED58A2-7205-4B5F-A73A-0426D86CF94C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>473867</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>140492</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDE63EFB-2A05-4716-A177-41155C538E26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2427,7 +4411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39340A3-B922-463C-8DD9-1D5D4A5D039E}">
   <dimension ref="B1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -3371,8 +5355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35398225-B916-4288-AEEF-908040A42457}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4259,109 +6243,109 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23">
-        <f xml:space="preserve"> AVERAGE(A2:A21)</f>
+        <f t="shared" ref="A23:M23" si="0" xml:space="preserve"> AVERAGE(A2:A21)</f>
         <v>-51.85</v>
       </c>
       <c r="B23">
-        <f xml:space="preserve"> AVERAGE(B2:B21)</f>
+        <f t="shared" si="0"/>
         <v>-52.55</v>
       </c>
       <c r="C23">
-        <f xml:space="preserve"> AVERAGE(C2:C21)</f>
+        <f t="shared" si="0"/>
         <v>-45.4</v>
       </c>
       <c r="D23">
-        <f xml:space="preserve"> AVERAGE(D2:D21)</f>
+        <f t="shared" si="0"/>
         <v>-43.7</v>
       </c>
       <c r="E23">
-        <f xml:space="preserve"> AVERAGE(E2:E21)</f>
+        <f t="shared" si="0"/>
         <v>-39.700000000000003</v>
       </c>
       <c r="F23">
-        <f xml:space="preserve"> AVERAGE(F2:F21)</f>
+        <f t="shared" si="0"/>
         <v>-37.9</v>
       </c>
       <c r="G23">
-        <f xml:space="preserve"> AVERAGE(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>-36.700000000000003</v>
       </c>
       <c r="H23">
-        <f xml:space="preserve"> AVERAGE(H2:H21)</f>
+        <f t="shared" si="0"/>
         <v>-35.200000000000003</v>
       </c>
       <c r="I23">
-        <f xml:space="preserve"> AVERAGE(I2:I21)</f>
+        <f t="shared" si="0"/>
         <v>-32.65</v>
       </c>
       <c r="J23">
-        <f xml:space="preserve"> AVERAGE(J2:J21)</f>
+        <f t="shared" si="0"/>
         <v>-23.85</v>
       </c>
       <c r="K23">
-        <f xml:space="preserve"> AVERAGE(K2:K21)</f>
+        <f t="shared" si="0"/>
         <v>-30.55</v>
       </c>
       <c r="L23">
-        <f xml:space="preserve"> AVERAGE(L2:L21)</f>
+        <f t="shared" si="0"/>
         <v>-20.5</v>
       </c>
       <c r="M23">
-        <f xml:space="preserve"> AVERAGE(M2:M21)</f>
+        <f t="shared" si="0"/>
         <v>-21.4</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
-        <f>10^(A23/10)</f>
+        <f t="shared" ref="A24:M24" si="1">10^(A23/10)</f>
         <v>6.5313055264747098E-6</v>
       </c>
       <c r="B24" s="3">
-        <f>10^(B23/10)</f>
+        <f t="shared" si="1"/>
         <v>5.5590425727040287E-6</v>
       </c>
       <c r="C24" s="3">
-        <f>10^(C23/10)</f>
+        <f t="shared" si="1"/>
         <v>2.8840315031266029E-5</v>
       </c>
       <c r="D24" s="3">
-        <f>10^(D23/10)</f>
+        <f t="shared" si="1"/>
         <v>4.265795188015923E-5</v>
       </c>
       <c r="E24" s="3">
-        <f>10^(E23/10)</f>
+        <f t="shared" si="1"/>
         <v>1.0715193052376051E-4</v>
       </c>
       <c r="F24" s="3">
-        <f>10^(F23/10)</f>
+        <f t="shared" si="1"/>
         <v>1.6218100973589279E-4</v>
       </c>
       <c r="G24" s="3">
-        <f>10^(G23/10)</f>
+        <f t="shared" si="1"/>
         <v>2.1379620895022272E-4</v>
       </c>
       <c r="H24" s="3">
-        <f>10^(H23/10)</f>
+        <f t="shared" si="1"/>
         <v>3.0199517204020104E-4</v>
       </c>
       <c r="I24" s="3">
-        <f>10^(I23/10)</f>
+        <f t="shared" si="1"/>
         <v>5.4325033149243333E-4</v>
       </c>
       <c r="J24" s="3">
-        <f>10^(J23/10)</f>
+        <f t="shared" si="1"/>
         <v>4.1209751909732969E-3</v>
       </c>
       <c r="K24" s="3">
-        <f>10^(K23/10)</f>
+        <f t="shared" si="1"/>
         <v>8.8104887300801315E-4</v>
       </c>
       <c r="L24" s="3">
-        <f>10^(L23/10)</f>
+        <f t="shared" si="1"/>
         <v>8.9125093813374554E-3</v>
       </c>
       <c r="M24" s="3">
-        <f>10^(M23/10)</f>
+        <f t="shared" si="1"/>
         <v>7.2443596007499E-3</v>
       </c>
       <c r="P24" s="3"/>
@@ -4531,6 +6515,1451 @@
       <c r="C38" s="2">
         <f>L24</f>
         <v>8.9125093813374554E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C9945-A92A-44C5-8AD1-1F8674DB4EAB}">
+  <dimension ref="A1:Q42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="9.265625" customWidth="1"/>
+    <col min="18" max="18" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>-50</v>
+      </c>
+      <c r="B2">
+        <v>-26</v>
+      </c>
+      <c r="C2">
+        <v>-30</v>
+      </c>
+      <c r="D2">
+        <v>-39</v>
+      </c>
+      <c r="E2">
+        <v>-29</v>
+      </c>
+      <c r="F2">
+        <v>-23</v>
+      </c>
+      <c r="G2">
+        <v>-18</v>
+      </c>
+      <c r="H2">
+        <v>-17</v>
+      </c>
+      <c r="I2">
+        <v>-14</v>
+      </c>
+      <c r="J2">
+        <v>-11</v>
+      </c>
+      <c r="K2">
+        <v>-12</v>
+      </c>
+      <c r="L2">
+        <v>-10</v>
+      </c>
+      <c r="M2">
+        <v>-11</v>
+      </c>
+      <c r="N2">
+        <v>-10</v>
+      </c>
+      <c r="O2">
+        <v>-10</v>
+      </c>
+      <c r="P2">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>-55</v>
+      </c>
+      <c r="B3">
+        <v>-30</v>
+      </c>
+      <c r="C3">
+        <v>-37</v>
+      </c>
+      <c r="D3">
+        <v>-39</v>
+      </c>
+      <c r="E3">
+        <v>-30</v>
+      </c>
+      <c r="F3">
+        <v>-22</v>
+      </c>
+      <c r="G3">
+        <v>-18</v>
+      </c>
+      <c r="H3">
+        <v>-17</v>
+      </c>
+      <c r="I3">
+        <v>-14</v>
+      </c>
+      <c r="J3">
+        <v>-11</v>
+      </c>
+      <c r="K3">
+        <v>-10</v>
+      </c>
+      <c r="L3">
+        <v>-10</v>
+      </c>
+      <c r="M3">
+        <v>-11</v>
+      </c>
+      <c r="N3">
+        <v>-10</v>
+      </c>
+      <c r="O3">
+        <v>-11</v>
+      </c>
+      <c r="P3">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>-51</v>
+      </c>
+      <c r="B4">
+        <v>-31</v>
+      </c>
+      <c r="C4">
+        <v>-32</v>
+      </c>
+      <c r="D4">
+        <v>-36</v>
+      </c>
+      <c r="E4">
+        <v>-30</v>
+      </c>
+      <c r="F4">
+        <v>-22</v>
+      </c>
+      <c r="G4">
+        <v>-18</v>
+      </c>
+      <c r="H4">
+        <v>-17</v>
+      </c>
+      <c r="I4">
+        <v>-14</v>
+      </c>
+      <c r="J4">
+        <v>-12</v>
+      </c>
+      <c r="K4">
+        <v>-11</v>
+      </c>
+      <c r="L4">
+        <v>-9</v>
+      </c>
+      <c r="M4">
+        <v>-12</v>
+      </c>
+      <c r="N4">
+        <v>-10</v>
+      </c>
+      <c r="O4">
+        <v>-11</v>
+      </c>
+      <c r="P4">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>-51</v>
+      </c>
+      <c r="B5">
+        <v>-31</v>
+      </c>
+      <c r="C5">
+        <v>-34</v>
+      </c>
+      <c r="D5">
+        <v>-36</v>
+      </c>
+      <c r="E5">
+        <v>-29</v>
+      </c>
+      <c r="F5">
+        <v>-23</v>
+      </c>
+      <c r="G5">
+        <v>-17</v>
+      </c>
+      <c r="H5">
+        <v>-17</v>
+      </c>
+      <c r="I5">
+        <v>-15</v>
+      </c>
+      <c r="J5">
+        <v>-11</v>
+      </c>
+      <c r="K5">
+        <v>-11</v>
+      </c>
+      <c r="L5">
+        <v>-10</v>
+      </c>
+      <c r="M5">
+        <v>-11</v>
+      </c>
+      <c r="N5">
+        <v>-10</v>
+      </c>
+      <c r="O5">
+        <v>-11</v>
+      </c>
+      <c r="P5">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>-51</v>
+      </c>
+      <c r="B6">
+        <v>-31</v>
+      </c>
+      <c r="C6">
+        <v>-37</v>
+      </c>
+      <c r="D6">
+        <v>-37</v>
+      </c>
+      <c r="E6">
+        <v>-29</v>
+      </c>
+      <c r="F6">
+        <v>-22</v>
+      </c>
+      <c r="G6">
+        <v>-17</v>
+      </c>
+      <c r="H6">
+        <v>-17</v>
+      </c>
+      <c r="I6">
+        <v>-13</v>
+      </c>
+      <c r="J6">
+        <v>-11</v>
+      </c>
+      <c r="K6">
+        <v>-12</v>
+      </c>
+      <c r="L6">
+        <v>-10</v>
+      </c>
+      <c r="M6">
+        <v>-11</v>
+      </c>
+      <c r="N6">
+        <v>-10</v>
+      </c>
+      <c r="O6">
+        <v>-11</v>
+      </c>
+      <c r="P6">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>-52</v>
+      </c>
+      <c r="B7">
+        <v>-31</v>
+      </c>
+      <c r="C7">
+        <v>-34</v>
+      </c>
+      <c r="D7">
+        <v>-40</v>
+      </c>
+      <c r="E7">
+        <v>-30</v>
+      </c>
+      <c r="F7">
+        <v>-22</v>
+      </c>
+      <c r="G7">
+        <v>-17</v>
+      </c>
+      <c r="H7">
+        <v>-17</v>
+      </c>
+      <c r="I7">
+        <v>-15</v>
+      </c>
+      <c r="J7">
+        <v>-11</v>
+      </c>
+      <c r="K7">
+        <v>-11</v>
+      </c>
+      <c r="L7">
+        <v>-10</v>
+      </c>
+      <c r="M7">
+        <v>-12</v>
+      </c>
+      <c r="N7">
+        <v>-11</v>
+      </c>
+      <c r="O7">
+        <v>-12</v>
+      </c>
+      <c r="P7">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>-52</v>
+      </c>
+      <c r="B8">
+        <v>-31</v>
+      </c>
+      <c r="C8">
+        <v>-35</v>
+      </c>
+      <c r="D8">
+        <v>-38</v>
+      </c>
+      <c r="E8">
+        <v>-30</v>
+      </c>
+      <c r="F8">
+        <v>-23</v>
+      </c>
+      <c r="G8">
+        <v>-18</v>
+      </c>
+      <c r="H8">
+        <v>-16</v>
+      </c>
+      <c r="I8">
+        <v>-14</v>
+      </c>
+      <c r="J8">
+        <v>-11</v>
+      </c>
+      <c r="K8">
+        <v>-11</v>
+      </c>
+      <c r="L8">
+        <v>-10</v>
+      </c>
+      <c r="M8">
+        <v>-12</v>
+      </c>
+      <c r="N8">
+        <v>-11</v>
+      </c>
+      <c r="O8">
+        <v>-11</v>
+      </c>
+      <c r="P8">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>-52</v>
+      </c>
+      <c r="B9">
+        <v>-31</v>
+      </c>
+      <c r="C9">
+        <v>-34</v>
+      </c>
+      <c r="D9">
+        <v>-37</v>
+      </c>
+      <c r="E9">
+        <v>-30</v>
+      </c>
+      <c r="F9">
+        <v>-23</v>
+      </c>
+      <c r="G9">
+        <v>-17</v>
+      </c>
+      <c r="H9">
+        <v>-16</v>
+      </c>
+      <c r="I9">
+        <v>-13</v>
+      </c>
+      <c r="J9">
+        <v>-11</v>
+      </c>
+      <c r="K9">
+        <v>-13</v>
+      </c>
+      <c r="L9">
+        <v>-10</v>
+      </c>
+      <c r="M9">
+        <v>-11</v>
+      </c>
+      <c r="N9">
+        <v>-10</v>
+      </c>
+      <c r="O9">
+        <v>-11</v>
+      </c>
+      <c r="P9">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>-53</v>
+      </c>
+      <c r="B10">
+        <v>-26</v>
+      </c>
+      <c r="C10">
+        <v>-34</v>
+      </c>
+      <c r="D10">
+        <v>-38</v>
+      </c>
+      <c r="E10">
+        <v>-29</v>
+      </c>
+      <c r="F10">
+        <v>-22</v>
+      </c>
+      <c r="G10">
+        <v>-18</v>
+      </c>
+      <c r="H10">
+        <v>-16</v>
+      </c>
+      <c r="I10">
+        <v>-13</v>
+      </c>
+      <c r="J10">
+        <v>-11</v>
+      </c>
+      <c r="K10">
+        <v>-11</v>
+      </c>
+      <c r="L10">
+        <v>-10</v>
+      </c>
+      <c r="M10">
+        <v>-11</v>
+      </c>
+      <c r="N10">
+        <v>-10</v>
+      </c>
+      <c r="O10">
+        <v>-12</v>
+      </c>
+      <c r="P10">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>-52</v>
+      </c>
+      <c r="B11">
+        <v>-31</v>
+      </c>
+      <c r="C11">
+        <v>-34</v>
+      </c>
+      <c r="D11">
+        <v>-37</v>
+      </c>
+      <c r="E11">
+        <v>-29</v>
+      </c>
+      <c r="F11">
+        <v>-22</v>
+      </c>
+      <c r="G11">
+        <v>-18</v>
+      </c>
+      <c r="H11">
+        <v>-16</v>
+      </c>
+      <c r="I11">
+        <v>-13</v>
+      </c>
+      <c r="J11">
+        <v>-10</v>
+      </c>
+      <c r="K11">
+        <v>-12</v>
+      </c>
+      <c r="L11">
+        <v>-10</v>
+      </c>
+      <c r="M11">
+        <v>-12</v>
+      </c>
+      <c r="N11">
+        <v>-10</v>
+      </c>
+      <c r="O11">
+        <v>-11</v>
+      </c>
+      <c r="P11">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>-51</v>
+      </c>
+      <c r="B12">
+        <v>-30</v>
+      </c>
+      <c r="C12">
+        <v>-34</v>
+      </c>
+      <c r="D12">
+        <v>-41</v>
+      </c>
+      <c r="E12">
+        <v>-30</v>
+      </c>
+      <c r="F12">
+        <v>-23</v>
+      </c>
+      <c r="G12">
+        <v>-19</v>
+      </c>
+      <c r="H12">
+        <v>-16</v>
+      </c>
+      <c r="I12">
+        <v>-14</v>
+      </c>
+      <c r="J12">
+        <v>-11</v>
+      </c>
+      <c r="K12">
+        <v>-12</v>
+      </c>
+      <c r="L12">
+        <v>-10</v>
+      </c>
+      <c r="M12">
+        <v>-11</v>
+      </c>
+      <c r="N12">
+        <v>-10</v>
+      </c>
+      <c r="O12">
+        <v>-11</v>
+      </c>
+      <c r="P12">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>-51</v>
+      </c>
+      <c r="B13">
+        <v>-30</v>
+      </c>
+      <c r="C13">
+        <v>-36</v>
+      </c>
+      <c r="D13">
+        <v>-38</v>
+      </c>
+      <c r="E13">
+        <v>-29</v>
+      </c>
+      <c r="F13">
+        <v>-23</v>
+      </c>
+      <c r="G13">
+        <v>-18</v>
+      </c>
+      <c r="H13">
+        <v>-16</v>
+      </c>
+      <c r="I13">
+        <v>-14</v>
+      </c>
+      <c r="J13">
+        <v>-11</v>
+      </c>
+      <c r="K13">
+        <v>-11</v>
+      </c>
+      <c r="L13">
+        <v>-10</v>
+      </c>
+      <c r="M13">
+        <v>-12</v>
+      </c>
+      <c r="N13">
+        <v>-10</v>
+      </c>
+      <c r="O13">
+        <v>-11</v>
+      </c>
+      <c r="P13">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>-51</v>
+      </c>
+      <c r="B14">
+        <v>-30</v>
+      </c>
+      <c r="C14">
+        <v>-39</v>
+      </c>
+      <c r="D14">
+        <v>-40</v>
+      </c>
+      <c r="E14">
+        <v>-29</v>
+      </c>
+      <c r="F14">
+        <v>-23</v>
+      </c>
+      <c r="G14">
+        <v>-17</v>
+      </c>
+      <c r="H14">
+        <v>-16</v>
+      </c>
+      <c r="I14">
+        <v>-15</v>
+      </c>
+      <c r="J14">
+        <v>-11</v>
+      </c>
+      <c r="K14">
+        <v>-12</v>
+      </c>
+      <c r="L14">
+        <v>-10</v>
+      </c>
+      <c r="M14">
+        <v>-11</v>
+      </c>
+      <c r="N14">
+        <v>-10</v>
+      </c>
+      <c r="O14">
+        <v>-11</v>
+      </c>
+      <c r="P14">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>-52</v>
+      </c>
+      <c r="B15">
+        <v>-26</v>
+      </c>
+      <c r="C15">
+        <v>-36</v>
+      </c>
+      <c r="D15">
+        <v>-37</v>
+      </c>
+      <c r="E15">
+        <v>-30</v>
+      </c>
+      <c r="F15">
+        <v>-23</v>
+      </c>
+      <c r="G15">
+        <v>-18</v>
+      </c>
+      <c r="H15">
+        <v>-16</v>
+      </c>
+      <c r="I15">
+        <v>-12</v>
+      </c>
+      <c r="J15">
+        <v>-12</v>
+      </c>
+      <c r="K15">
+        <v>-11</v>
+      </c>
+      <c r="L15">
+        <v>-9</v>
+      </c>
+      <c r="M15">
+        <v>-11</v>
+      </c>
+      <c r="N15">
+        <v>-9</v>
+      </c>
+      <c r="O15">
+        <v>-11</v>
+      </c>
+      <c r="P15">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>-52</v>
+      </c>
+      <c r="B16">
+        <v>-25</v>
+      </c>
+      <c r="C16">
+        <v>-38</v>
+      </c>
+      <c r="D16">
+        <v>-40</v>
+      </c>
+      <c r="E16">
+        <v>-29</v>
+      </c>
+      <c r="F16">
+        <v>-23</v>
+      </c>
+      <c r="G16">
+        <v>-18</v>
+      </c>
+      <c r="H16">
+        <v>-16</v>
+      </c>
+      <c r="I16">
+        <v>-13</v>
+      </c>
+      <c r="J16">
+        <v>-12</v>
+      </c>
+      <c r="K16">
+        <v>-13</v>
+      </c>
+      <c r="L16">
+        <v>-9</v>
+      </c>
+      <c r="M16">
+        <v>-11</v>
+      </c>
+      <c r="N16">
+        <v>-10</v>
+      </c>
+      <c r="O16">
+        <v>-11</v>
+      </c>
+      <c r="P16">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>-52</v>
+      </c>
+      <c r="B17">
+        <v>-29</v>
+      </c>
+      <c r="C17">
+        <v>-35</v>
+      </c>
+      <c r="D17">
+        <v>-37</v>
+      </c>
+      <c r="E17">
+        <v>-29</v>
+      </c>
+      <c r="F17">
+        <v>-23</v>
+      </c>
+      <c r="G17">
+        <v>-18</v>
+      </c>
+      <c r="H17">
+        <v>-16</v>
+      </c>
+      <c r="I17">
+        <v>-13</v>
+      </c>
+      <c r="J17">
+        <v>-12</v>
+      </c>
+      <c r="K17">
+        <v>-11</v>
+      </c>
+      <c r="L17">
+        <v>-9</v>
+      </c>
+      <c r="M17">
+        <v>-12</v>
+      </c>
+      <c r="N17">
+        <v>-10</v>
+      </c>
+      <c r="O17">
+        <v>-10</v>
+      </c>
+      <c r="P17">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>-52</v>
+      </c>
+      <c r="B18">
+        <v>-25</v>
+      </c>
+      <c r="C18">
+        <v>-34</v>
+      </c>
+      <c r="D18">
+        <v>-41</v>
+      </c>
+      <c r="E18">
+        <v>-30</v>
+      </c>
+      <c r="F18">
+        <v>-22</v>
+      </c>
+      <c r="G18">
+        <v>-18</v>
+      </c>
+      <c r="H18">
+        <v>-16</v>
+      </c>
+      <c r="I18">
+        <v>-12</v>
+      </c>
+      <c r="J18">
+        <v>-12</v>
+      </c>
+      <c r="K18">
+        <v>-11</v>
+      </c>
+      <c r="L18">
+        <v>-10</v>
+      </c>
+      <c r="M18">
+        <v>-12</v>
+      </c>
+      <c r="N18">
+        <v>-10</v>
+      </c>
+      <c r="O18">
+        <v>-10</v>
+      </c>
+      <c r="P18">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>-52</v>
+      </c>
+      <c r="B19">
+        <v>-25</v>
+      </c>
+      <c r="C19">
+        <v>-36</v>
+      </c>
+      <c r="D19">
+        <v>-39</v>
+      </c>
+      <c r="E19">
+        <v>-30</v>
+      </c>
+      <c r="F19">
+        <v>-21</v>
+      </c>
+      <c r="G19">
+        <v>-17</v>
+      </c>
+      <c r="H19">
+        <v>-16</v>
+      </c>
+      <c r="I19">
+        <v>-12</v>
+      </c>
+      <c r="J19">
+        <v>-12</v>
+      </c>
+      <c r="K19">
+        <v>-12</v>
+      </c>
+      <c r="L19">
+        <v>-11</v>
+      </c>
+      <c r="M19">
+        <v>-11</v>
+      </c>
+      <c r="N19">
+        <v>-11</v>
+      </c>
+      <c r="O19">
+        <v>-10</v>
+      </c>
+      <c r="P19">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>-53</v>
+      </c>
+      <c r="B20">
+        <v>-25</v>
+      </c>
+      <c r="C20">
+        <v>-36</v>
+      </c>
+      <c r="D20">
+        <v>-37</v>
+      </c>
+      <c r="E20">
+        <v>-29</v>
+      </c>
+      <c r="F20">
+        <v>-22</v>
+      </c>
+      <c r="G20">
+        <v>-18</v>
+      </c>
+      <c r="H20">
+        <v>-16</v>
+      </c>
+      <c r="I20">
+        <v>-12</v>
+      </c>
+      <c r="J20">
+        <v>-12</v>
+      </c>
+      <c r="K20">
+        <v>-12</v>
+      </c>
+      <c r="L20">
+        <v>-11</v>
+      </c>
+      <c r="M20">
+        <v>-12</v>
+      </c>
+      <c r="N20">
+        <v>-10</v>
+      </c>
+      <c r="O20">
+        <v>-11</v>
+      </c>
+      <c r="P20">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>-52</v>
+      </c>
+      <c r="B21">
+        <v>-30</v>
+      </c>
+      <c r="C21">
+        <v>-35</v>
+      </c>
+      <c r="D21">
+        <v>-40</v>
+      </c>
+      <c r="E21">
+        <v>-24</v>
+      </c>
+      <c r="F21">
+        <v>-22</v>
+      </c>
+      <c r="G21">
+        <v>-18</v>
+      </c>
+      <c r="H21">
+        <v>-16</v>
+      </c>
+      <c r="I21">
+        <v>-12</v>
+      </c>
+      <c r="J21">
+        <v>-12</v>
+      </c>
+      <c r="K21">
+        <v>-11</v>
+      </c>
+      <c r="L21">
+        <v>-11</v>
+      </c>
+      <c r="M21">
+        <v>-11</v>
+      </c>
+      <c r="N21">
+        <v>-9</v>
+      </c>
+      <c r="O21">
+        <v>-10</v>
+      </c>
+      <c r="P21">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <f t="shared" ref="A23:M23" si="0" xml:space="preserve"> AVERAGE(A2:A21)</f>
+        <v>-51.85</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>-28.7</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-35</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-38.35</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>-29.2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>-22.45</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>-17.75</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>-16.3</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>-13.35</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>-11.35</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:O23" si="1" xml:space="preserve"> AVERAGE(L2:L21)</f>
+        <v>-9.9499999999999993</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>-11.4</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>-10.050000000000001</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>-10.85</v>
+      </c>
+      <c r="P23">
+        <f xml:space="preserve"> AVERAGE(P2:P21)</f>
+        <v>-10.95</v>
+      </c>
+      <c r="Q23" t="e">
+        <f xml:space="preserve"> AVERAGE(Q2:Q21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A24" s="3">
+        <f t="shared" ref="A24:M24" si="2">10^(A23/10)</f>
+        <v>6.5313055264747098E-6</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3489628825916523E-3</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1622776601683783E-4</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4621771744567172E-4</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2022644346174124E-3</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>5.6885293084384106E-3</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6788040181225605E-2</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="2"/>
+        <v>2.3442288153199212E-2</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="2"/>
+        <v>4.6238102139926025E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="2"/>
+        <v>7.3282453313890383E-2</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="2"/>
+        <v>7.0794578438413788E-2</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" ref="L24" si="3">10^(L23/10)</f>
+        <v>0.10115794542598987</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" ref="M24" si="4">10^(M23/10)</f>
+        <v>7.2443596007498959E-2</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" ref="N24" si="5">10^(N23/10)</f>
+        <v>9.8855309465693833E-2</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" ref="O24" si="6">10^(O23/10)</f>
+        <v>8.2224264994707086E-2</v>
+      </c>
+      <c r="P24" s="3">
+        <f>10^(P23/10)</f>
+        <v>8.03526122185617E-2</v>
+      </c>
+      <c r="Q24" s="3" t="e">
+        <f>10^(Q23/10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" s="5">
+        <f>A23</f>
+        <v>-51.85</v>
+      </c>
+      <c r="C27" s="6">
+        <f>A24</f>
+        <v>6.5313055264747098E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5">
+        <f>B23</f>
+        <v>-28.7</v>
+      </c>
+      <c r="C28" s="6">
+        <f>B24</f>
+        <v>1.3489628825916523E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5">
+        <f>C23</f>
+        <v>-35</v>
+      </c>
+      <c r="C29" s="6">
+        <f>C24</f>
+        <v>3.1622776601683783E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5">
+        <f>D23</f>
+        <v>-38.35</v>
+      </c>
+      <c r="C30" s="6">
+        <f>D24</f>
+        <v>1.4621771744567172E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" s="5">
+        <f>E23</f>
+        <v>-29.2</v>
+      </c>
+      <c r="C31" s="6">
+        <f>E24</f>
+        <v>1.2022644346174124E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5">
+        <f>F23</f>
+        <v>-22.45</v>
+      </c>
+      <c r="C32" s="6">
+        <f>F24</f>
+        <v>5.6885293084384106E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" s="5">
+        <f>G23</f>
+        <v>-17.75</v>
+      </c>
+      <c r="C33" s="6">
+        <f>G24</f>
+        <v>1.6788040181225605E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" s="5">
+        <f>H23</f>
+        <v>-16.3</v>
+      </c>
+      <c r="C34" s="6">
+        <f>H24</f>
+        <v>2.3442288153199212E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" s="5">
+        <f>I23</f>
+        <v>-13.35</v>
+      </c>
+      <c r="C35" s="6">
+        <f>I24</f>
+        <v>4.6238102139926025E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5">
+        <f>J23</f>
+        <v>-11.35</v>
+      </c>
+      <c r="C36" s="6">
+        <f>J24</f>
+        <v>7.3282453313890383E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37" s="5">
+        <f>K23</f>
+        <v>-11.5</v>
+      </c>
+      <c r="C37" s="6">
+        <f>K24</f>
+        <v>7.0794578438413788E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38" s="5">
+        <f>L23</f>
+        <v>-9.9499999999999993</v>
+      </c>
+      <c r="C38" s="7">
+        <f>L24</f>
+        <v>0.10115794542598987</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" s="5">
+        <f>M23</f>
+        <v>-11.4</v>
+      </c>
+      <c r="C39" s="7">
+        <f>M24</f>
+        <v>7.2443596007498959E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40" s="5">
+        <f>N23</f>
+        <v>-10.050000000000001</v>
+      </c>
+      <c r="C40" s="7">
+        <f>N24</f>
+        <v>9.8855309465693833E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41" s="5">
+        <f>O23</f>
+        <v>-10.85</v>
+      </c>
+      <c r="C41" s="7">
+        <f>O24</f>
+        <v>8.2224264994707086E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42" s="1">
+        <f>P23</f>
+        <v>-10.95</v>
+      </c>
+      <c r="C42" s="2">
+        <f>P24</f>
+        <v>8.03526122185617E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>